<commit_message>
feat: created new table
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>Öğrenci</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Şube</t>
   </si>
   <si>
-    <t>10/A</t>
-  </si>
-  <si>
     <t>11/B</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>12/B</t>
   </si>
   <si>
-    <t>9/C</t>
-  </si>
-  <si>
     <t>06.12.2004</t>
   </si>
   <si>
@@ -141,7 +135,22 @@
     <t>Fen</t>
   </si>
   <si>
-    <t>Kimya</t>
+    <t>Şube Adı</t>
+  </si>
+  <si>
+    <t>11/A</t>
+  </si>
+  <si>
+    <t>12/A</t>
+  </si>
+  <si>
+    <t>Edebiyat</t>
+  </si>
+  <si>
+    <t>Ders</t>
+  </si>
+  <si>
+    <t>Programlama Temelleri</t>
   </si>
 </sst>
 </file>
@@ -195,13 +204,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,17 +912,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
   </cols>
@@ -970,8 +982,8 @@
       <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" t="s">
-        <v>23</v>
+      <c r="H3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -996,8 +1008,8 @@
       <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" t="s">
-        <v>24</v>
+      <c r="H4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1005,7 +1017,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1020,10 +1032,10 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
         <v>27</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1031,10 +1043,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6">
         <v>103</v>
@@ -1046,15 +1058,15 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
         <v>28</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1080,7 +1092,7 @@
         <v>22</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1088,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -1102,11 +1114,11 @@
       <c r="F10" t="s">
         <v>15</v>
       </c>
-      <c r="G10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" t="s">
-        <v>35</v>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1114,7 +1126,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1128,11 +1140,11 @@
       <c r="F11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" t="s">
-        <v>36</v>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1140,7 +1152,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1152,13 +1164,13 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" t="s">
         <v>27</v>
       </c>
-      <c r="H12" t="s">
-        <v>37</v>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1166,7 +1178,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1178,13 +1190,150 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" t="s">
         <v>28</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: done school database
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>Öğrenci</t>
   </si>
@@ -151,6 +151,21 @@
   </si>
   <si>
     <t>Programlama Temelleri</t>
+  </si>
+  <si>
+    <t>Şube Id</t>
+  </si>
+  <si>
+    <t>Branş Id</t>
+  </si>
+  <si>
+    <t>Şube-Öğretmen</t>
+  </si>
+  <si>
+    <t>Öğretmen Id</t>
+  </si>
+  <si>
+    <t>Ders Id</t>
   </si>
 </sst>
 </file>
@@ -914,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,7 +972,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1089,10 +1104,10 @@
         <v>7</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1203,6 +1218,9 @@
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1213,45 +1231,87 @@
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
@@ -1259,7 +1319,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1267,7 +1327,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1275,7 +1335,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1283,7 +1343,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
@@ -1291,12 +1351,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>1</v>
       </c>
@@ -1304,7 +1364,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1312,7 +1372,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>

</xml_diff>